<commit_message>
implementado pdf y excel en libro de caja
</commit_message>
<xml_diff>
--- a/public/reporte.xlsx
+++ b/public/reporte.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+  <si>
+    <t>SALDO ANT</t>
+  </si>
   <si>
     <t>NRO</t>
   </si>
@@ -41,7 +44,7 @@
     <t>CONCEPTO</t>
   </si>
   <si>
-    <t>2025-03-01</t>
+    <t>2025-04-01</t>
   </si>
   <si>
     <t>Ingreso</t>
@@ -50,22 +53,22 @@
     <t>Haber</t>
   </si>
   <si>
-    <t>Saldo Inicial</t>
-  </si>
-  <si>
-    <t>saldo inicial de la iglesia monte de sion</t>
-  </si>
-  <si>
-    <t>2025-03-03</t>
-  </si>
-  <si>
-    <t>Ofrenda misionera</t>
-  </si>
-  <si>
-    <t>ofrendas</t>
-  </si>
-  <si>
-    <t>2025-03-05</t>
+    <t>Diezmo anterior</t>
+  </si>
+  <si>
+    <t>Raquel Uceda - diezmo de marzo</t>
+  </si>
+  <si>
+    <t>2025-04-04</t>
+  </si>
+  <si>
+    <t>Diezmo actual</t>
+  </si>
+  <si>
+    <t>Alberto Oriz - diezmo</t>
+  </si>
+  <si>
+    <t>2025-04-16</t>
   </si>
   <si>
     <t>Egreso</t>
@@ -74,28 +77,22 @@
     <t>Debe</t>
   </si>
   <si>
+    <t>Compra de flores para el Altar</t>
+  </si>
+  <si>
+    <t>compra de flores</t>
+  </si>
+  <si>
+    <t>2025-04-29</t>
+  </si>
+  <si>
     <t>Capacitación</t>
   </si>
   <si>
-    <t>capacitacion al sistema</t>
-  </si>
-  <si>
-    <t>2025-03-20</t>
-  </si>
-  <si>
-    <t>Atención a Visitantes</t>
-  </si>
-  <si>
-    <t>atencion a visitantes de iglesias</t>
-  </si>
-  <si>
-    <t>2025-03-23</t>
-  </si>
-  <si>
-    <t>Ofrenda niños E. dominical</t>
-  </si>
-  <si>
-    <t>ofrenda de niños</t>
+    <t>clases de canto</t>
+  </si>
+  <si>
+    <t>Ofrenda recogida</t>
   </si>
 </sst>
 </file>
@@ -435,7 +432,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,194 +442,176 @@
   <cols>
     <col min="1" max="1" width="4.57" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="23.423" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="6.998" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="4.57" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="31.707" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="49.417" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="36.42" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="36.42" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>3000.0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>140</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
+      <c r="C1">
+        <v>2992.69999999999982</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
-        <v>150.0</v>
+      <c r="C3" t="s">
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>754</v>
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>120.5</v>
+        <v>100.0</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>150.0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>751</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
         <v>16</v>
-      </c>
-      <c r="C5">
-        <v>200.0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5">
-        <v>624</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>50.0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6">
+        <v>656</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
         <v>21</v>
-      </c>
-      <c r="C6">
-        <v>80.0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6">
-        <v>625</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>85.0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7">
+        <v>624</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
         <v>24</v>
       </c>
-      <c r="C7">
-        <v>2.2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>12.0</v>
+      </c>
+      <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="F7">
-        <v>756</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8">
+        <v>753</v>
+      </c>
+      <c r="G8" t="s">
         <v>25</v>
       </c>
-      <c r="H7" t="s">
-        <v>26</v>
+      <c r="H8" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>